<commit_message>
Added 2024 MLR Round 17 forecasts
</commit_message>
<xml_diff>
--- a/seasons/RugbyUnion/MajorLeagueRugby/2024/forecasts/ReportRound10.xlsx
+++ b/seasons/RugbyUnion/MajorLeagueRugby/2024/forecasts/ReportRound10.xlsx
@@ -109,6 +109,24 @@
     <t>Germantown, MD</t>
   </si>
   <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>San Diego, CA</t>
+  </si>
+  <si>
+    <t>UTAH</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>Herriman, UT</t>
+  </si>
+  <si>
     <t>NE</t>
   </si>
   <si>
@@ -116,24 +134,6 @@
   </si>
   <si>
     <t>Quincy, MA</t>
-  </si>
-  <si>
-    <t>UTAH</t>
-  </si>
-  <si>
-    <t>HOU</t>
-  </si>
-  <si>
-    <t>Herriman, UT</t>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>DAL</t>
-  </si>
-  <si>
-    <t>San Diego, CA</t>
   </si>
 </sst>
 </file>
@@ -189,7 +189,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFC81A2E"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1E191A"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -213,15 +221,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF1E191A"/>
+      <color rgb="FFC81A2E"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -268,13 +268,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF031E41"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00653C"/>
+        <fgColor rgb="FF00AE94"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,13 +292,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF031E41"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00AE94"/>
+        <fgColor rgb="FF00653C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,19 +347,19 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -755,23 +755,23 @@
         <v>1</v>
       </c>
       <c r="B3" s="13">
-        <v>0.4241462287477051</v>
+        <v>0.4392988685458171</v>
       </c>
       <c r="C3" s="13"/>
       <c r="E3" s="13">
-        <v>0.3671493321915389</v>
+        <v>0.3539143270102322</v>
       </c>
       <c r="F3" s="13"/>
       <c r="H3" s="13">
-        <v>0.7568119377357776</v>
+        <v>0.6106098076875619</v>
       </c>
       <c r="I3" s="13"/>
       <c r="K3" s="13">
-        <v>0.7065931436128716</v>
+        <v>0.6327904855701001</v>
       </c>
       <c r="L3" s="13"/>
       <c r="N3" s="13">
-        <v>0.5530120890181276</v>
+        <v>0.6984511870276118</v>
       </c>
       <c r="O3" s="13"/>
     </row>
@@ -780,23 +780,23 @@
         <v>2</v>
       </c>
       <c r="B4" s="13">
-        <v>0.1931270146317139</v>
+        <v>0.1844651940891014</v>
       </c>
       <c r="C4" s="13"/>
       <c r="E4" s="13">
-        <v>0.9872112670390765</v>
+        <v>0.9863154541264124</v>
       </c>
       <c r="F4" s="13"/>
       <c r="H4" s="13">
-        <v>0.9633300747248524</v>
+        <v>0.9750484611273017</v>
       </c>
       <c r="I4" s="13"/>
       <c r="K4" s="13">
-        <v>0.8871692721590488</v>
+        <v>0.8819861617716395</v>
       </c>
       <c r="L4" s="13"/>
       <c r="N4" s="13">
-        <v>0.9760772683555728</v>
+        <v>0.9607097032292017</v>
       </c>
       <c r="O4" s="13"/>
     </row>
@@ -805,23 +805,23 @@
         <v>3</v>
       </c>
       <c r="B5" s="12">
-        <v>8.191409492534431</v>
+        <v>8.103535104942678</v>
       </c>
       <c r="C5" s="12"/>
       <c r="E5" s="12">
-        <v>36.24539574253599</v>
+        <v>34.90711701669408</v>
       </c>
       <c r="F5" s="12"/>
       <c r="H5" s="12">
-        <v>72.9059700531667</v>
+        <v>59.53741533349948</v>
       </c>
       <c r="I5" s="12"/>
       <c r="K5" s="12">
-        <v>62.68677249316055</v>
+        <v>55.81124515735846</v>
       </c>
       <c r="L5" s="12"/>
       <c r="N5" s="12">
-        <v>53.97825292164229</v>
+        <v>67.10088326093806</v>
       </c>
       <c r="O5" s="12"/>
     </row>
@@ -830,34 +830,34 @@
         <v>4</v>
       </c>
       <c r="B6" s="14">
-        <v>0.9702518999999999</v>
+        <v>0.9683138</v>
       </c>
       <c r="C6" s="14">
-        <v>0.0297481</v>
+        <v>0.0279348</v>
       </c>
       <c r="E6" s="14">
-        <v>0.4335235</v>
+        <v>0.419787</v>
       </c>
       <c r="F6" s="14">
-        <v>0.5664765</v>
+        <v>0.5536506</v>
       </c>
       <c r="H6" s="14">
-        <v>0.6122532000000001</v>
+        <v>0.397784</v>
       </c>
       <c r="I6" s="14">
-        <v>0.3877468</v>
+        <v>0.5789078</v>
       </c>
       <c r="K6" s="14">
-        <v>0.3048755</v>
+        <v>0.2935928</v>
       </c>
       <c r="L6" s="14">
-        <v>0.6951245</v>
+        <v>0.683195</v>
       </c>
       <c r="N6" s="14">
-        <v>0.4091977</v>
+        <v>0.6001646</v>
       </c>
       <c r="O6" s="14">
-        <v>0.5908023</v>
+        <v>0.3738772</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -865,34 +865,34 @@
         <v>5</v>
       </c>
       <c r="B7" s="15">
-        <v>52.8474886</v>
+        <v>52.8498334</v>
       </c>
       <c r="C7" s="15">
-        <v>15.9727844</v>
+        <v>15.9739616</v>
       </c>
       <c r="E7" s="15">
-        <v>21.5448018</v>
+        <v>21.5311834</v>
       </c>
       <c r="F7" s="15">
-        <v>24.237715</v>
+        <v>24.2327876</v>
       </c>
       <c r="H7" s="15">
-        <v>30.2894536</v>
+        <v>24.7969314</v>
       </c>
       <c r="I7" s="15">
-        <v>24.9545346</v>
+        <v>28.7979424</v>
       </c>
       <c r="K7" s="15">
-        <v>21.4194878</v>
+        <v>21.4212702</v>
       </c>
       <c r="L7" s="15">
-        <v>30.4313612</v>
+        <v>30.4208194</v>
       </c>
       <c r="N7" s="15">
-        <v>24.796169</v>
+        <v>30.3037918</v>
       </c>
       <c r="O7" s="15">
-        <v>28.8035352</v>
+        <v>24.9389478</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -912,10 +912,10 @@
         <v>7</v>
       </c>
       <c r="H8" s="15">
+        <v>7</v>
+      </c>
+      <c r="I8" s="15">
         <v>10</v>
-      </c>
-      <c r="I8" s="15">
-        <v>7</v>
       </c>
       <c r="K8" s="15">
         <v>5</v>
@@ -924,10 +924,10 @@
         <v>10</v>
       </c>
       <c r="N8" s="15">
+        <v>10</v>
+      </c>
+      <c r="O8" s="15">
         <v>7</v>
-      </c>
-      <c r="O8" s="15">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -947,10 +947,10 @@
         <v>10</v>
       </c>
       <c r="H9" s="15">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I9" s="15">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K9" s="15">
         <v>8</v>
@@ -959,10 +959,10 @@
         <v>14</v>
       </c>
       <c r="N9" s="15">
+        <v>14</v>
+      </c>
+      <c r="O9" s="15">
         <v>10</v>
-      </c>
-      <c r="O9" s="15">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -982,10 +982,10 @@
         <v>12</v>
       </c>
       <c r="H10" s="15">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I10" s="15">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K10" s="15">
         <v>10</v>
@@ -994,10 +994,10 @@
         <v>17</v>
       </c>
       <c r="N10" s="15">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="O10" s="15">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1017,10 +1017,10 @@
         <v>14</v>
       </c>
       <c r="H11" s="15">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I11" s="15">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K11" s="15">
         <v>12</v>
@@ -1029,10 +1029,10 @@
         <v>19</v>
       </c>
       <c r="N11" s="15">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="O11" s="15">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1052,10 +1052,10 @@
         <v>16</v>
       </c>
       <c r="H12" s="15">
+        <v>16</v>
+      </c>
+      <c r="I12" s="15">
         <v>20</v>
-      </c>
-      <c r="I12" s="15">
-        <v>16</v>
       </c>
       <c r="K12" s="15">
         <v>13</v>
@@ -1064,10 +1064,10 @@
         <v>21</v>
       </c>
       <c r="N12" s="15">
+        <v>20</v>
+      </c>
+      <c r="O12" s="15">
         <v>16</v>
-      </c>
-      <c r="O12" s="15">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1087,10 +1087,10 @@
         <v>17</v>
       </c>
       <c r="H13" s="15">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I13" s="15">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K13" s="15">
         <v>15</v>
@@ -1099,10 +1099,10 @@
         <v>22</v>
       </c>
       <c r="N13" s="15">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="O13" s="15">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1122,10 +1122,10 @@
         <v>19</v>
       </c>
       <c r="H14" s="15">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I14" s="15">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="K14" s="15">
         <v>17</v>
@@ -1134,10 +1134,10 @@
         <v>24</v>
       </c>
       <c r="N14" s="15">
+        <v>24</v>
+      </c>
+      <c r="O14" s="15">
         <v>19</v>
-      </c>
-      <c r="O14" s="15">
-        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1157,10 +1157,10 @@
         <v>20</v>
       </c>
       <c r="H15" s="15">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I15" s="15">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K15" s="15">
         <v>17</v>
@@ -1169,10 +1169,10 @@
         <v>26</v>
       </c>
       <c r="N15" s="15">
+        <v>26</v>
+      </c>
+      <c r="O15" s="15">
         <v>21</v>
-      </c>
-      <c r="O15" s="15">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1192,10 +1192,10 @@
         <v>22</v>
       </c>
       <c r="H16" s="15">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I16" s="15">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="K16" s="15">
         <v>19</v>
@@ -1204,10 +1204,10 @@
         <v>28</v>
       </c>
       <c r="N16" s="15">
+        <v>27</v>
+      </c>
+      <c r="O16" s="15">
         <v>22</v>
-      </c>
-      <c r="O16" s="15">
-        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1227,10 +1227,10 @@
         <v>23</v>
       </c>
       <c r="H17" s="15">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I17" s="15">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="K17" s="15">
         <v>20</v>
@@ -1239,10 +1239,10 @@
         <v>29</v>
       </c>
       <c r="N17" s="15">
+        <v>29</v>
+      </c>
+      <c r="O17" s="15">
         <v>24</v>
-      </c>
-      <c r="O17" s="15">
-        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1262,10 +1262,10 @@
         <v>25</v>
       </c>
       <c r="H18" s="15">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="I18" s="15">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K18" s="15">
         <v>22</v>
@@ -1274,10 +1274,10 @@
         <v>31</v>
       </c>
       <c r="N18" s="15">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="O18" s="15">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1297,10 +1297,10 @@
         <v>26</v>
       </c>
       <c r="H19" s="15">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I19" s="15">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K19" s="15">
         <v>24</v>
@@ -1309,10 +1309,10 @@
         <v>33</v>
       </c>
       <c r="N19" s="15">
+        <v>33</v>
+      </c>
+      <c r="O19" s="15">
         <v>27</v>
-      </c>
-      <c r="O19" s="15">
-        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1332,10 +1332,10 @@
         <v>28</v>
       </c>
       <c r="H20" s="15">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I20" s="15">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K20" s="15">
         <v>25</v>
@@ -1344,10 +1344,10 @@
         <v>35</v>
       </c>
       <c r="N20" s="15">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="O20" s="15">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1367,10 +1367,10 @@
         <v>30</v>
       </c>
       <c r="H21" s="15">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="I21" s="15">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="K21" s="15">
         <v>27</v>
@@ -1379,10 +1379,10 @@
         <v>37</v>
       </c>
       <c r="N21" s="15">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="O21" s="15">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1402,10 +1402,10 @@
         <v>32</v>
       </c>
       <c r="H22" s="15">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I22" s="15">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="K22" s="15">
         <v>29</v>
@@ -1414,10 +1414,10 @@
         <v>39</v>
       </c>
       <c r="N22" s="15">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="O22" s="15">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1437,10 +1437,10 @@
         <v>34</v>
       </c>
       <c r="H23" s="15">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I23" s="15">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="K23" s="15">
         <v>31</v>
@@ -1449,10 +1449,10 @@
         <v>41</v>
       </c>
       <c r="N23" s="15">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="O23" s="15">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1472,10 +1472,10 @@
         <v>36</v>
       </c>
       <c r="H24" s="15">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="I24" s="15">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="K24" s="15">
         <v>33</v>
@@ -1484,10 +1484,10 @@
         <v>45</v>
       </c>
       <c r="N24" s="15">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="O24" s="15">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1507,10 +1507,10 @@
         <v>40</v>
       </c>
       <c r="H25" s="15">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="I25" s="15">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="K25" s="15">
         <v>36</v>
@@ -1519,10 +1519,10 @@
         <v>48</v>
       </c>
       <c r="N25" s="15">
+        <v>48</v>
+      </c>
+      <c r="O25" s="15">
         <v>41</v>
-      </c>
-      <c r="O25" s="15">
-        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -1542,10 +1542,10 @@
         <v>45</v>
       </c>
       <c r="H26" s="15">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="I26" s="15">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="K26" s="15">
         <v>41</v>
@@ -1554,10 +1554,10 @@
         <v>55</v>
       </c>
       <c r="N26" s="15">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="O26" s="15">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>